<commit_message>
TD-6649 add Business Concept file manager domain name field
</commit_message>
<xml_diff>
--- a/test/fixtures/incorrect_upload.xlsx
+++ b/test/fixtures/incorrect_upload.xlsx
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">domain</t>
+    <t xml:space="preserve">domain_external_id</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
     <t xml:space="preserve">critical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domain</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
@@ -112,12 +115,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,49 +141,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>